<commit_message>
log updates, and most recent licor files uploaded
</commit_message>
<xml_diff>
--- a/logs/water_fertilizer_shuffle_mk.xlsx
+++ b/logs/water_fertilizer_shuffle_mk.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monik\Documents\git\2025_g34p\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BEA96A-F2C7-433A-8161-CD18B2A92646}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D444A78-27A2-4FA9-ADCB-1C1749E9C32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="31">
   <si>
     <t>date</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>shuffled all</t>
+  </si>
+  <si>
+    <t>thanks Zarra</t>
   </si>
 </sst>
 </file>
@@ -468,22 +471,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="77.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="77.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -500,7 +503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45847</v>
       </c>
@@ -518,12 +521,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45848</v>
       </c>
       <c r="B3" s="5">
-        <f t="shared" ref="B3:B37" si="0">A3</f>
+        <f t="shared" ref="B3:B40" si="0">A3</f>
         <v>45848</v>
       </c>
       <c r="C3" t="s">
@@ -536,7 +539,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>45851</v>
       </c>
@@ -554,7 +557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>45852</v>
       </c>
@@ -572,7 +575,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>45854</v>
       </c>
@@ -590,7 +593,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>45856</v>
       </c>
@@ -608,7 +611,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>45860</v>
       </c>
@@ -626,7 +629,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>45863</v>
       </c>
@@ -644,7 +647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>45863</v>
       </c>
@@ -662,7 +665,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>45870</v>
       </c>
@@ -680,7 +683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>45870</v>
       </c>
@@ -698,7 +701,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45870</v>
       </c>
@@ -716,7 +719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45870</v>
       </c>
@@ -734,7 +737,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45873</v>
       </c>
@@ -752,7 +755,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45873</v>
       </c>
@@ -770,7 +773,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45876</v>
       </c>
@@ -788,7 +791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45876</v>
       </c>
@@ -806,7 +809,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>45880</v>
       </c>
@@ -824,7 +827,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>45881</v>
       </c>
@@ -842,7 +845,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>45881</v>
       </c>
@@ -860,7 +863,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>45883</v>
       </c>
@@ -878,7 +881,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>45884</v>
       </c>
@@ -896,7 +899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>45887</v>
       </c>
@@ -914,7 +917,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>45889</v>
       </c>
@@ -932,7 +935,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>45891</v>
       </c>
@@ -950,7 +953,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>45894</v>
       </c>
@@ -968,7 +971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>45905</v>
       </c>
@@ -986,7 +989,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>45906</v>
       </c>
@@ -1004,7 +1007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>45907</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>45903</v>
       </c>
@@ -1040,7 +1043,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>45907</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>45909</v>
       </c>
@@ -1076,7 +1079,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>45917</v>
       </c>
@@ -1094,7 +1097,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>45916</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>45913</v>
       </c>
@@ -1127,7 +1130,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>45919</v>
       </c>
@@ -1143,6 +1146,54 @@
       </c>
       <c r="E37" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>45927</v>
+      </c>
+      <c r="B38" s="5">
+        <f t="shared" si="0"/>
+        <v>45927</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>45928</v>
+      </c>
+      <c r="B39" s="5">
+        <f t="shared" si="0"/>
+        <v>45928</v>
+      </c>
+      <c r="C39" t="s">
+        <v>18</v>
+      </c>
+      <c r="D39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>45931</v>
+      </c>
+      <c r="B40" s="5">
+        <f t="shared" si="0"/>
+        <v>45931</v>
+      </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>